<commit_message>
update to timeline and added project requirementes
</commit_message>
<xml_diff>
--- a/Docs/Time_Line.xlsx
+++ b/Docs/Time_Line.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Time Line</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t xml:space="preserve">Architectural Planning and Planning the Tech Stack</t>
+  </si>
+  <si>
+    <t>Auth_Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database 1st Draft</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -124,32 +130,94 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right/>
+      <right style="none"/>
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
       <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -160,64 +228,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -276,29 +291,35 @@
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,109 +908,158 @@
       </c>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" ht="42.75">
-      <c r="A7" s="20" t="s">
+    <row r="7" ht="16.5">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" ht="16.5">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" ht="42.75">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21">
-        <v>46028</v>
-      </c>
-      <c r="C7" s="21">
-        <v>46028</v>
-      </c>
-      <c r="D7" s="21">
+      <c r="B9" s="22">
+        <v>46028</v>
+      </c>
+      <c r="C9" s="22">
+        <v>46028</v>
+      </c>
+      <c r="D9" s="22">
         <v>46038</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" ht="28.5">
-      <c r="A8" s="20" t="s">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="28.5">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="21">
-        <v>46028</v>
-      </c>
-      <c r="C8" s="21">
-        <v>46028</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="B10" s="22">
+        <v>46028</v>
+      </c>
+      <c r="C10" s="22">
+        <v>46028</v>
+      </c>
+      <c r="D10" s="22">
         <v>46071</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="21">
-        <v>46028</v>
-      </c>
-      <c r="C11" s="21">
-        <v>46028</v>
-      </c>
-      <c r="D11" s="21">
-        <v>46028</v>
-      </c>
-      <c r="E11" s="21">
-        <v>46028</v>
-      </c>
-    </row>
-    <row r="12" ht="28.5">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="22">
+        <v>46028</v>
+      </c>
+      <c r="C13" s="22">
+        <v>46028</v>
+      </c>
+      <c r="D13" s="22">
+        <v>46028</v>
+      </c>
+      <c r="E13" s="22">
+        <v>46028</v>
+      </c>
+    </row>
+    <row r="14" ht="28.5">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="21">
-        <v>46028</v>
-      </c>
-      <c r="C12" s="21">
-        <v>46028</v>
-      </c>
-      <c r="D12" s="21">
-        <v>46028</v>
-      </c>
-      <c r="E12" s="21">
+      <c r="B14" s="22">
+        <v>46028</v>
+      </c>
+      <c r="C14" s="22">
+        <v>46028</v>
+      </c>
+      <c r="D14" s="22">
+        <v>46028</v>
+      </c>
+      <c r="E14" s="22">
         <v>46029</v>
       </c>
     </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+    <row r="15" ht="14.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="22">
+        <v>46029</v>
+      </c>
+      <c r="C17" s="22">
+        <v>46029</v>
+      </c>
+      <c r="D17" s="22">
+        <v>46036</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="22">
+        <v>46028</v>
+      </c>
+      <c r="C18" s="22">
+        <v>46028</v>
+      </c>
+      <c r="D18" s="22">
+        <v>46030</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:F3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A9:F10"/>
+    <mergeCell ref="A7:F8"/>
+    <mergeCell ref="A11:F12"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Update to time linhe and project requerements
</commit_message>
<xml_diff>
--- a/Docs/Time_Line.xlsx
+++ b/Docs/Time_Line.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Time Line</t>
   </si>
@@ -57,13 +57,22 @@
     <t xml:space="preserve">Architectural Planning and Planning the Tech Stack</t>
   </si>
   <si>
+    <t xml:space="preserve">Had to be changed later</t>
+  </si>
+  <si>
     <t>Auth_Services</t>
   </si>
   <si>
+    <t xml:space="preserve">Login with google and password changes/recovery toke way longer then expected.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Database 1st Draft</t>
   </si>
   <si>
     <t xml:space="preserve">Database Final Version</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t xml:space="preserve">RestAPI with all fetures and functionalaty</t>
@@ -85,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -119,16 +128,34 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="7" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -244,29 +271,11 @@
       </bottom>
       <diagonal style="none"/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -277,9 +286,6 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -314,7 +320,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -344,6 +350,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -352,6 +367,12 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,16 +380,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,112 +901,112 @@
     <col customWidth="1" min="1" max="1" style="1" width="27.7109375"/>
     <col customWidth="1" min="2" max="5" style="2" width="14.7109375"/>
     <col min="6" max="6" style="3" width="9.140625"/>
-    <col customWidth="1" min="7" max="7" style="4" width="51.421875"/>
+    <col customWidth="1" min="7" max="7" style="1" width="51.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" ht="48.75" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" ht="16.5">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" ht="16.5">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" ht="16.5">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" ht="16.5">
-      <c r="A7" s="22"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" ht="16.5">
-      <c r="A8" s="22"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" ht="42.75">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>46028</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <v>46028</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>46038</v>
       </c>
       <c r="E9" s="2"/>
@@ -1003,49 +1015,49 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>46028</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="22">
         <v>46028</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>46071</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>46028</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="22">
         <v>46028</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>46028</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>46028</v>
       </c>
     </row>
@@ -1053,196 +1065,207 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>46028</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="22">
         <v>46028</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <v>46028</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="26">
         <v>46029</v>
       </c>
+      <c r="G14" s="27" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-    </row>
-    <row r="17" ht="14.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" ht="28.5">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="23">
+        <v>14</v>
+      </c>
+      <c r="B17" s="22">
         <v>46029</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="22">
         <v>46029</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <v>46036</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="28">
+        <v>46043</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="23">
+        <v>16</v>
+      </c>
+      <c r="B18" s="22">
         <v>46028</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <v>46028</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>46030</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>46030</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="28">
+      <c r="A19" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="30">
         <v>46030</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28">
+      <c r="C19" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="30">
         <v>46043</v>
       </c>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="23">
+        <v>19</v>
+      </c>
+      <c r="B22" s="22">
         <v>46036</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <v>46050</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="23">
+        <v>20</v>
+      </c>
+      <c r="B25" s="22">
         <v>46036</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <v>46057</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="23">
+        <v>21</v>
+      </c>
+      <c r="B26" s="22">
         <v>46055</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <v>46069</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="23">
+        <v>22</v>
+      </c>
+      <c r="B29" s="22">
         <v>46065</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="22">
         <v>46071</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Update to Teck Stack used. Update to DB to include isDeleted field to solft delete data
</commit_message>
<xml_diff>
--- a/Docs/Time_Line.xlsx
+++ b/Docs/Time_Line.xlsx
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Architectural Planning and Planning the Tech Stack</t>
   </si>
   <si>
-    <t xml:space="preserve">Had to be changed later</t>
+    <t xml:space="preserve">Had to be changed later (22-1-2026)</t>
   </si>
   <si>
     <t>Auth_Services</t>
@@ -72,10 +72,10 @@
     <t xml:space="preserve">Database Final Version</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t xml:space="preserve">RestAPI with all fetures and functionalaty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delay on start caused by login taking too long.</t>
   </si>
   <si>
     <t>WebSite</t>
@@ -367,7 +367,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="5" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1143,8 +1143,8 @@
       <c r="B19" s="30">
         <v>46030</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>18</v>
+      <c r="C19" s="31">
+        <v>46044</v>
       </c>
       <c r="D19" s="30">
         <v>46043</v>
@@ -1171,13 +1171,19 @@
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="22">
         <v>46036</v>
       </c>
+      <c r="C22" s="28">
+        <v>46044</v>
+      </c>
       <c r="D22" s="22">
         <v>46050</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" ht="14.25">

</xml_diff>

<commit_message>
Added Courses and modules. update to DB small bug fix update to time_line
</commit_message>
<xml_diff>
--- a/Docs/Time_Line.xlsx
+++ b/Docs/Time_Line.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">Time Line</t>
   </si>
@@ -45,7 +45,37 @@
     <t>Ended</t>
   </si>
   <si>
-    <t xml:space="preserve">Part 1: Login Fully working with Google and Facebook as Auth methods</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Part 1: Login Fully working with Google and </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Facebook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as Auth methods</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fully working with Google</t>
   </si>
   <si>
     <t xml:space="preserve">Part 2: Project fully complete and working</t>
@@ -72,13 +102,88 @@
     <t xml:space="preserve">Database Final Version</t>
   </si>
   <si>
-    <t xml:space="preserve">RestAPI with all fetures and functionalaty</t>
+    <t>RestAPI</t>
   </si>
   <si>
     <t xml:space="preserve">Delay on start caused by login taking too long.</t>
   </si>
   <si>
+    <t xml:space="preserve">Users (base)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70% -  falta separar entre Formadores e Alunos</t>
+  </si>
+  <si>
+    <t>Cursos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40% falta adicionar, adicionar modulos e editar </t>
+  </si>
+  <si>
+    <t>Modulos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70% falta editar</t>
+  </si>
+  <si>
+    <t>Turmas</t>
+  </si>
+  <si>
+    <t>Salas</t>
+  </si>
+  <si>
+    <t>Horarios</t>
+  </si>
+  <si>
+    <t>Disponibilidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relação Formadores turma modulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creiação de Horarios automáticos</t>
+  </si>
+  <si>
     <t>WebSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login 2FA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagina home para alunos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagina home para Formadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagina para gerir users geral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80% Precisa de polimento, mas está funcional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagina para gerir Alunos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Página para gerir Formadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcação de diponibilidade para formadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcção de disponibilidade para salas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat Bot</t>
   </si>
   <si>
     <t xml:space="preserve">Mobile APP (android)</t>
@@ -135,12 +240,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -150,12 +261,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -178,104 +289,11 @@
       </bottom>
       <diagonal style="none"/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -286,34 +304,10 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -322,65 +316,38 @@
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="5" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,373 +875,658 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" ht="48.75" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" ht="16.5">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" ht="16.5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" ht="16.5">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" ht="16.5">
-      <c r="A7" s="21"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" ht="16.5">
-      <c r="A8" s="21"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" ht="42.75">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="9">
         <v>46028</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="9">
         <v>46028</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="9">
         <v>46038</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="10">
+        <v>46043</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" ht="28.5">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="22">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
         <v>46028</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="9">
         <v>46028</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="9">
         <v>46071</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9">
         <v>46028</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="9">
         <v>46028</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="9">
         <v>46028</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="9">
         <v>46028</v>
       </c>
     </row>
     <row r="14" ht="28.5">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="22">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9">
         <v>46028</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="9">
         <v>46028</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="9">
         <v>46028</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="11">
         <v>46029</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>13</v>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" ht="28.5">
       <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="22">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
         <v>46029</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="9">
         <v>46029</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="9">
         <v>46036</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="10">
         <v>46043</v>
       </c>
-      <c r="G17" s="27" t="s">
-        <v>15</v>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="22">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9">
         <v>46028</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="9">
         <v>46028</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="9">
         <v>46030</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="9">
         <v>46030</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="30">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9">
         <v>46030</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="10">
         <v>46044</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="9">
         <v>46043</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" ht="28.5">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="22">
+      <c r="A22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9">
         <v>46036</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="10">
         <v>46044</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="9">
         <v>46050</v>
       </c>
-      <c r="G22" s="27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="22">
+    </row>
+    <row r="23" ht="28.5">
+      <c r="A23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" ht="28.5">
+      <c r="A24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" ht="28.5">
+      <c r="A25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="G25" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" ht="28.5">
+      <c r="A26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="28.5">
+      <c r="A27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="28.5">
+      <c r="A28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="28.5">
+      <c r="A29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="28.5">
+      <c r="A30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="28.5">
+      <c r="A31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9">
         <v>46036</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D34" s="9">
         <v>46057</v>
       </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="22">
+      <c r="E34" s="2"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="G36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="G37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="G38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="G39" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="G40" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" ht="28.5">
+      <c r="A44" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="G44" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" ht="28.5">
+      <c r="A45" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="G45" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="G46" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" ht="14.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="9">
         <v>46055</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D49" s="9">
         <v>46069</v>
       </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="22">
+      <c r="G49" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" ht="14.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" ht="14.25">
+      <c r="A52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="9">
         <v>46065</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D52" s="9">
         <v>46071</v>
       </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-    </row>
-    <row r="31" ht="14.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
+      <c r="G52" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="56" ht="28.5"/>
+    <row r="57" ht="28.5"/>
+    <row r="64" ht="14.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="A1:G3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:E4"/>
@@ -1285,9 +1537,11 @@
     <mergeCell ref="A11:G12"/>
     <mergeCell ref="A15:G16"/>
     <mergeCell ref="A20:G21"/>
-    <mergeCell ref="A23:G24"/>
-    <mergeCell ref="A27:G28"/>
-    <mergeCell ref="A30:G31"/>
+    <mergeCell ref="A32:G33"/>
+    <mergeCell ref="A47:G48"/>
+    <mergeCell ref="A50:G51"/>
+    <mergeCell ref="A53:G54"/>
+    <mergeCell ref="A64:G65"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>

</xml_diff>